<commit_message>
gantt als png added
</commit_message>
<xml_diff>
--- a/slides/BSP23_Gantt.xlsx
+++ b/slides/BSP23_Gantt.xlsx
@@ -208,8 +208,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="75">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -348,6 +350,7 @@
     <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -384,6 +387,7 @@
     <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -716,13 +720,15 @@
   <dimension ref="B3:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="A2" sqref="A2:T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="19" width="4.6640625" customWidth="1"/>
+    <col min="20" max="20" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:23">

</xml_diff>